<commit_message>
simple crawling with excel
</commit_message>
<xml_diff>
--- a/tmp.xlsx
+++ b/tmp.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="상품정보" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,28 +413,1143 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="80" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>data1</t>
+          <t>상품명: 보몽드 순면스퀘어 솔리드 누빔매트커버, 다크블루</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>data2</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>data3</t>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>상품명: 슈에뜨룸 선인장 리플 침구 세트, 베이지</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>상품명: 선우랜드 레인보우 2단 문걸이용 옷걸이 _중형, 화이트, 상세페이지참조</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>상품명: 보드래 헬로우 누빔 매트리스커버, 핑크</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>상품명: 보드래 퍼펙트 누빔 매트리스커버, 차콜</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>상품명: 피아블 클래식 방수 매트리스커버, 화이트</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>상품명: 더자리 에코항균 마이크로 매트리스커버, 밀키차콜그레이</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>상품명: 더자리 프레쉬 퓨어 매트리스 커버, 퓨어 차콜그레이</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>상품명: 몽쉐어 알러스킨 항균 매트리스 커버, 카키그레이</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>상품명: 쿠팡 브랜드 - 코멧 홈 40수 트윌 순면 100% 홑겹 매트리스커버, 그레이</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>상품명: 패브릭아트 항균 마이크로 원단 매트리스 커버, 아이보리</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>상품명: 바숨 순면 누빔 침대 매트리스커버, 차콜</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>상품명: WEMAX 다용도 문옷걸이, 화이트, 1개</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>상품명: 타카타카 프리미엄 나노 화이바 누빔 매트리스 커버, 젠틀핑핑</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>상품명: 보몽드 순면스퀘어 누빔매트커버, 다크그레이</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>상품명: 보드래 국내산 순면 60수 누빔 매트리스커버, 그레이</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>상품명: 보드래 퍼펙트 누빔 매트리스커버, 베이지핑크</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>상품명: 쿠팡 브랜드 - 코멧 홈 40수 순면 누빔 매트리스커버, 챠콜</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>상품명: 바숨 순면 누빔 침대 매트리스커버, 화이트</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>상품명: 프랑떼 항균 방수 매트리스커버, 화이트</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>상품명: 보몽드 순면스퀘어 솔리드 누빔매트커버, 다크블루</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>상품명: 네이쳐리빙 피아블 클래식 방수 매트리스커버, 그레이</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>상품명: 쿠팡 브랜드 - 코멧 홈 순면 매트리스커버, 베이지</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>상품명: 타카타카 프리미엄 나노 화이바 누빔 매트리스 커버, 프렌치불독</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>상품명: 더자리 에코항균 마이크로 매트리스커버, 밀키그레이</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>상품명: 보몽드 순면스퀘어 누빔매트커버, 화이트</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>상품명: 피아블 클래식 방수 매트리스커버, 화이트</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>상품명: 쿠팡 브랜드 - 코멧 홈 순면 매트리스커버, 차콜그레이</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>상품명: 쉬즈홈 모던그리드 순면 여름이불 베개커버 패드세트, 핑크</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>상품명: 스코홈 빅리플 여름 차렵이불패드 3종 세트, 마린그레이</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>상품명: 아망떼 시어서커 리플 홑이불 패드세트, 웨이크</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>상품명: 마이센스 무더운 여름엔 시어서커 여름이불 패드 베개 이불세트 30종, 시어서커_파스텔그레이</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>상품명: 믹스앤매치 로라 프릴 시어서커 침구세트, 그레이</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>상품명: 에피소드1 샤베트 프릴 시어서커 여름이불패드세트, 그레이</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>상품명: 슈에뜨룸 선인장 리플 침구 세트, 베이지</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>상품명: 아망떼 시어서커 리플 홑이불 패드세트, 허브티</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>상품명: 지베딩 아이스베어 시어서커 여름침구 풀세트, 민트그레이</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>상품명: 쁘리엘르 테스 시어서커 여름이불 패드세트, 그레이</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>상품명: 쉬즈홈 시어서커 홑이불 + 토퍼 + 베개커버 세트, 나나 옐로우</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>상품명: 아망떼 시어서커 리플 퀼팅 이불패드세트, 리엔나</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>상품명: 바자르 트로피컬 인견 여름 이불세트 인견이불 + 베개커버 2p + 인견패드, 그린</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>상품명: 바자르 라이닝 혼방 인견 여름 이불베개세트 + 패드 Q, 쿨 네이비</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>상품명: 슈에뜨룸 비숑 피치스킨 침구세트, 그레이</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>상품명: 스코홈 시어서커 여름 이불 패드 3종 세트, 차콜</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>상품명: 스코홈 어번시리즈 순면 차렵이불 누빔 매트커버세트 S 차콜</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>상품명: 쉬즈홈 루즈 시어서커 차렵이불 패드세트, 그레이</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>상품명: 예가로드 메리엘 시어서커 누비이불 패드세트, 블루</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>상품명: 에피소드1 샤베트 프릴 시어서커 여름이불패드세트, 화이트</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>상품명: 쉬즈홈 플루 시어서커 차렵이불 패드세트, 그린</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>상품명: 메종 레이스 차렵 이불 세트, 블루</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>상품명: 믹스앤매치 로라 프릴 시어서커 침구세트, 그린</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>상품명: 슈에뜨룸 발그레 피치 리플 침구 세트, 혼합 색상</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>상품명: 보몽드 메종 레이스 차렵이불 3종 세트, 민트</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>상품명: 슈에뜨룸 체크 피치스킨 침구세트, 모카</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>상품명: 메리엘 시어서커 에어리플 이불세트, 그레이</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>상품명: 슈에뜨룸 빠삐용 시어서커 침구세트, 네이비</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>상품명: 믹스앤매치 에이프릴 리플 누비이불 패드세트, 화이트</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>상품명: 쉬즈홈 시어서커 홑이불 토퍼세트, 루즈 그레이</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>상품명: 이코디 5단 엔틱 도어 행거, 브라운, 1개</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>상품명: 선우랜드 우드볼 도어훅 4구, 실버, 1개</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>상품명: 리은상점 다용도 도어훅 문걸이 행거 모자걸이 머플러 목도리 걸이, 화이트, 5개</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>상품명: 퍼니스코 다용도걸이 모자걸이 가방걸이 도어훅 도어행거 문걸이, 엔틱브라운, 1세트</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>상품명: 스텐 도어후크 옷걸이/도어훅 문옷걸이 행거 바지걸이, 혼합 색상, 1개</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>상품명: 디비플러스 키펙스 컬러 폭조절 오버 도어훅, 블랙, 1개</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>상품명: 리빙스토리 1+1 문에 거는 문 옷걸이 음자리 도어후크 방문 행거, 음자리도어후크-로즈골드, 2개</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>상품명: 나이스후크 도어행거 2개 세트 (문행거), 블랙+화이트</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>상품명: 리빙파이 도어훅 옷걸이 행거 7구, 블랙, 1개</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>상품명: 선우랜드 우드볼 도어훅 10구, 실버, 1개</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>상품명: 웰렉스 도어행거 MH1060 신형 본사직발송 미니건조대 도어옷걸이 도어훅, 고동색, 1개</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>상품명: 엔비 엔틱 7구 도어훅 옷걸이, 도어훅 1+1, 1+1</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>상품명: 코시나 무타공 문걸이 후크선반 1단, 화이트, 1개</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>상품명: 코시나 무타공 올스텐 문걸이행거, 혼합 색상, 1개</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>상품명: [아트박스 POOM/이케아] ENUDDEN 도어 행거, 본품, 수량</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>상품명: 비스비바 우드 폴 다용도걸이 3구, 혼합 색상, 1개</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>상품명: 숲속애 웨이브 도어후크 5구, 블랙, 1개</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>상품명: 펀타스틱 다용도 문틀걸이, 화이트, 1개</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>상품명: 선우랜드 우드볼 도어훅 4구, 화이트, 1개</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>상품명: 네이쳐리빙 어반모카 와이어 도어훅 옷걸이 6구, 단일 색상, 1개</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>상품명: 까사마루 블랑 접이식 문걸이 건조대, 1개</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>상품명: 선우랜드 우드볼 도어훅 6구, 실버, 1개</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>상품명: 이케아 ENUDDEN 문걸이 행거 402.516.66, 화이트, 1개</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>상품명: 선우랜드 우드볼 도어훅 10구, 화이트, 1개</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>상품명: 코멧 홈 우드볼 도어행거, 6구, 혼합색상</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>상품명: 선우랜드 레인보우 2단 문걸이용 옷걸이 _중형, 화이트, 상세페이지참조</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>상품명: 코시나 무타공 문걸이 후크선반 2단, 화이트, 1개</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>상품명: 스파이더락 도어후크 8구, 화이트, 1개</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>상품명: 선우랜드 우드볼 도어훅 6구, 화이트, 1개</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>상품명: 코멧 홈 우드볼 도어행거, 10구, 혼합색상</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>상품명: 보드래 헬로우 누빔 매트리스커버, 핑크</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>상품명: 보몽드 순면스퀘어 솔리드 누빔매트커버, 아이보리</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>상품명: 더자리 에코항균 마이크로 매트리스커버, 밀키핑크</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>상품명: 타카타카 프리미엄 나노 화이바 누빔 매트리스 커버, 미스밍고</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>상품명: 네이쳐리빙 피아블 클래식 방수 매트리스커버, 그레이</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>상품명: 프로텍트어베드 베이직 매트리스 방수커버, 그레이</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>05 Jun 2020</t>
         </is>
       </c>
     </row>

</xml_diff>